<commit_message>
Update TestJson.xlsx for ScopePropertiesMiddleware tests
</commit_message>
<xml_diff>
--- a/test/EDennis.AspNetCore.MiddlewareTests/EDennis.AspNetCore.MiddlewareTests/ScopeProperties/TestJson.xlsx
+++ b/test/EDennis.AspNetCore.MiddlewareTests/EDennis.AspNetCore.MiddlewareTests/ScopeProperties/TestJson.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MitchellDenC\source\repos\EDennis.AspNetCore.Base\test\EDennis.AspNetCore.MiddlewareTests\EDennis.AspNetCore.MiddlewareTests\ScopeProperties\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DB3299-2480-42F2-92A1-904D0A90D0F9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA05C0E-917B-452C-8000-C91A9708540F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
   </bookViews>
@@ -60,17 +60,9 @@
     <t>Expected</t>
   </si>
   <si>
-    <t>{"FirstName":"Moe","LastName":"Stooge"
-}</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
-    <t>{"FirstName":"Larry","LastName":"Stooge"
-}</t>
-  </si>
-  <si>
     <t>Get</t>
   </si>
   <si>
@@ -83,9 +75,6 @@
     <t>Claims</t>
   </si>
   <si>
-    <t>claim*group=123&amp;claim*role=admin</t>
-  </si>
-  <si>
     <t>Headers</t>
   </si>
   <si>
@@ -95,7 +84,16 @@
     <t>claim*role=user&amp;claim*group=456</t>
   </si>
   <si>
-    <t>header*hdr1=123&amp;header*hdr2=456</t>
+    <t>claim*name=jack&amp;claim*role=admin</t>
+  </si>
+  <si>
+    <t>header*hdr1=123&amp;header*x-user=jill</t>
+  </si>
+  <si>
+    <t>{"User":"jack","Claims":[{"Type":"name","Value":"jack"},{"Type":"role","Value":"admin"}],"Headers":{"hdr1":["ABC"],"hdr2":["DEF"]}}</t>
+  </si>
+  <si>
+    <t>{"User":"jill","Claims":[{"Type":"role","Value":"user"},{"Type":"group","Value":"456"}],"Headers":{"hdr1":["123"],"x-user":["jill"]}}</t>
   </si>
 </sst>
 </file>
@@ -451,7 +449,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,53 +489,53 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
@@ -546,67 +544,67 @@
         <v>8</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>